<commit_message>
Split the scenarios, added clean up, and logic for job run and control table updates
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_AZ_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_AZ_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -88,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +100,14 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,18 +115,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -405,20 +443,20 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -449,20 +487,20 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>20000101</v>
       </c>
-      <c r="E2" s="3">
-        <v>0</v>
+      <c r="E2" s="2">
+        <v>20180630</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -470,16 +508,16 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>20180701</v>
+      </c>
+      <c r="E3" s="2">
         <v>99999999</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Johns Commit 1: Control table expiration date change
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_AZ_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_AZ_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -443,20 +443,20 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -491,7 +491,7 @@
         <v>20000101</v>
       </c>
       <c r="E2" s="2">
-        <v>20180630</v>
+        <v>20181201</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -500,7 +500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -509,7 +509,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>20180701</v>
+        <v>20181202</v>
       </c>
       <c r="E3" s="2">
         <v>99999999</v>

</xml_diff>